<commit_message>
2003 Hate Crimes refresh
</commit_message>
<xml_diff>
--- a/ope.ed.gov/2003/hate-crimes-noncampus-virginia-colleges-and-universities-crime-2003.xlsx
+++ b/ope.ed.gov/2003/hate-crimes-noncampus-virginia-colleges-and-universities-crime-2003.xlsx
@@ -13,16 +13,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t>Hate Crimes - Noncampus</t>
-  </si>
-  <si>
-    <t>Survey year</t>
-  </si>
-  <si>
-    <t>Unitid</t>
-  </si>
-  <si>
-    <t>Institution name</t>
+    <t>Survey Year</t>
+  </si>
+  <si>
+    <t>UnitID</t>
+  </si>
+  <si>
+    <t>Institution Name</t>
   </si>
   <si>
     <t>Campus ID</t>
@@ -34,88 +31,88 @@
     <t>Institution Size</t>
   </si>
   <si>
-    <t>Murder/Non-negligent manslaughter</t>
-  </si>
-  <si>
-    <t>Murder/Non-negligent manslaughter - Race</t>
-  </si>
-  <si>
-    <t>Murder/Non-negligent manslaughter - Religion</t>
-  </si>
-  <si>
-    <t>Murder/Non-negligent manslaughter - Sexual orientation</t>
-  </si>
-  <si>
-    <t>Murder/Non-negligent manslaughter - Gender</t>
-  </si>
-  <si>
-    <t>Murder/Non-negligent manslaughter - Disability</t>
-  </si>
-  <si>
-    <t>Murder/Non-negligent manslaughter - Ethnicity/National origin</t>
-  </si>
-  <si>
-    <t>Negligent manslaughter</t>
-  </si>
-  <si>
-    <t>Negligent manslaughter - Race</t>
-  </si>
-  <si>
-    <t>Negligent manslaughter - Religion</t>
-  </si>
-  <si>
-    <t>Negligent manslaughter - Sexual orientation</t>
-  </si>
-  <si>
-    <t>Negligent manslaughter - Gender</t>
-  </si>
-  <si>
-    <t>Negligent manslaughter - Disability</t>
-  </si>
-  <si>
-    <t>Negligent manslaughter - Ethnicity/National origin</t>
-  </si>
-  <si>
-    <t>Sex offenses - Forcible</t>
-  </si>
-  <si>
-    <t>Sex offenses - Forcible - Race</t>
-  </si>
-  <si>
-    <t>Sex offenses - Forcible - Religion</t>
-  </si>
-  <si>
-    <t>Sex offenses - Forcible - Sexual orientation</t>
-  </si>
-  <si>
-    <t>Sex offenses - Forcible - Gender</t>
-  </si>
-  <si>
-    <t>Sex offenses - Forcible - Disability</t>
-  </si>
-  <si>
-    <t>Sex offenses - Forcible - Ethnicity/National origin</t>
-  </si>
-  <si>
-    <t>Sex offenses - Non-forcible</t>
-  </si>
-  <si>
-    <t>Sex offenses - Non-forcible -Race</t>
-  </si>
-  <si>
-    <t>Sex offenses - Non-forcible - Religion</t>
-  </si>
-  <si>
-    <t>Sex offenses - Non-forcible - Sexual orientation</t>
-  </si>
-  <si>
-    <t>Sex offenses - Non-forcible - Gender</t>
-  </si>
-  <si>
-    <t>Sex offenses - Non-forcible - Disability</t>
-  </si>
-  <si>
-    <t>Sex offenses - Non-forcible - Ethnicity/National origin</t>
+    <t>Murder/Non-Negligent Manslaughter</t>
+  </si>
+  <si>
+    <t>Murder/Non-Negligent Manslaughter - Race</t>
+  </si>
+  <si>
+    <t>Murder/Non-Negligent Manslaughter - Religion</t>
+  </si>
+  <si>
+    <t>Murder/Non-Negligent Manslaughter - Sexual Orientation</t>
+  </si>
+  <si>
+    <t>Murder/Non-Negligent Manslaughter - Gender</t>
+  </si>
+  <si>
+    <t>Murder/Non-Negligent Manslaughter - Disability</t>
+  </si>
+  <si>
+    <t>Murder/Non-Negligent Manslaughter - Ethnicity/National Origin</t>
+  </si>
+  <si>
+    <t>Negligent Manslaughter</t>
+  </si>
+  <si>
+    <t>Negligent Manslaughter - Race</t>
+  </si>
+  <si>
+    <t>Negligent Manslaughter - Religion</t>
+  </si>
+  <si>
+    <t>Negligent Manslaughter - Sexual Orientation</t>
+  </si>
+  <si>
+    <t>Negligent Manslaughter - Gender</t>
+  </si>
+  <si>
+    <t>Negligent Manslaughter - Disability</t>
+  </si>
+  <si>
+    <t>Negligent Manslaughter - Ethnicity/National Origin</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Forcible</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Forcible - Race</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Forcible - Religion</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Forcible - Sexual Orientation</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Forcible - Gender</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Forcible - Disability</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Forcible - Ethnicity/National Origin</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Non-Forcible</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Non-Forcible -Race</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Non-Forcible - Religion</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Non-Forcible - Sexual Orientation</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Non-Forcible - Gender</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Non-Forcible - Disability</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Non-Forcible - Ethnicity/National Origin</t>
   </si>
   <si>
     <t>Robbery</t>
@@ -127,7 +124,7 @@
     <t>Robbery - Religion</t>
   </si>
   <si>
-    <t>Robbery - Sexual orientation</t>
+    <t>Robbery - Sexual Orientation</t>
   </si>
   <si>
     <t>Robbery - Gender</t>
@@ -136,28 +133,28 @@
     <t>Robbery - Disability</t>
   </si>
   <si>
-    <t>Robbery - Ethnicity/National origin</t>
-  </si>
-  <si>
-    <t>Aggravated assault</t>
-  </si>
-  <si>
-    <t>Aggravated assault - Race</t>
-  </si>
-  <si>
-    <t>Aggravated assault - Religion</t>
-  </si>
-  <si>
-    <t>Aggravated assault - Sexual orientation</t>
-  </si>
-  <si>
-    <t>Aggravated assault - Gender</t>
-  </si>
-  <si>
-    <t>Aggravated assault - Disability</t>
-  </si>
-  <si>
-    <t>Aggravated assault - Ethnicity/National origin</t>
+    <t>Robbery - Ethnicity/National Origin</t>
+  </si>
+  <si>
+    <t>Aggravated Assault</t>
+  </si>
+  <si>
+    <t>Aggravated Assault - Race</t>
+  </si>
+  <si>
+    <t>Aggravated Assault - Religion</t>
+  </si>
+  <si>
+    <t>Aggravated Assault - Sexual Orientation</t>
+  </si>
+  <si>
+    <t>Aggravated Assault - Gender</t>
+  </si>
+  <si>
+    <t>Aggravated Assault - Disability</t>
+  </si>
+  <si>
+    <t>Aggravated Assault - Ethnicity/National Origin</t>
   </si>
   <si>
     <t>Burglary</t>
@@ -169,7 +166,7 @@
     <t>Burglary - Religion</t>
   </si>
   <si>
-    <t>Burglary - Sexual orientation</t>
+    <t>Burglary - Sexual Orientation</t>
   </si>
   <si>
     <t>Burglary - Gender</t>
@@ -178,28 +175,28 @@
     <t>Burglary - Disability</t>
   </si>
   <si>
-    <t>Burglary - Ethnicity/National origin</t>
-  </si>
-  <si>
-    <t>Motor vehicle theft</t>
-  </si>
-  <si>
-    <t>Motor vehicle theft - Race</t>
-  </si>
-  <si>
-    <t>Motor vehicle theft - Religion</t>
-  </si>
-  <si>
-    <t>Motor vehicle theft - Sexual orientation</t>
-  </si>
-  <si>
-    <t>Motor vehicle theft - Gender</t>
-  </si>
-  <si>
-    <t>Motor vehicle theft - Disability</t>
-  </si>
-  <si>
-    <t>Motor vehicle theft - Ethnicity/National origin</t>
+    <t>Burglary - Ethnicity/National Origin</t>
+  </si>
+  <si>
+    <t>Motor Vehicle Theft</t>
+  </si>
+  <si>
+    <t>Motor Vehicle Theft - Race</t>
+  </si>
+  <si>
+    <t>Motor Vehicle Theft - Religion</t>
+  </si>
+  <si>
+    <t>Motor Vehicle Theft - Sexual Orientation</t>
+  </si>
+  <si>
+    <t>Motor Vehicle Theft - Gender</t>
+  </si>
+  <si>
+    <t>Motor Vehicle Theft - Disability</t>
+  </si>
+  <si>
+    <t>Motor Vehicle Theft - Ethnicity/National Origin</t>
   </si>
   <si>
     <t>Arson</t>
@@ -211,7 +208,7 @@
     <t>Arson - Religion</t>
   </si>
   <si>
-    <t>Arson - Sexual orientation</t>
+    <t>Arson - Sexual Orientation</t>
   </si>
   <si>
     <t>Arson - Gender</t>
@@ -220,49 +217,49 @@
     <t>Arson - Disability</t>
   </si>
   <si>
-    <t>Arson - Ethnicity/National origin</t>
-  </si>
-  <si>
-    <t>Simple assault</t>
-  </si>
-  <si>
-    <t>Simple assault - Race</t>
-  </si>
-  <si>
-    <t>Simple assault - Religion</t>
-  </si>
-  <si>
-    <t>Simple assault - Sexual orientation</t>
-  </si>
-  <si>
-    <t>Simple assault - Gender</t>
-  </si>
-  <si>
-    <t>Simple assault - Disability</t>
-  </si>
-  <si>
-    <t>Simple assault - Ethnicity/National origin</t>
-  </si>
-  <si>
-    <t>Larceny-theft</t>
-  </si>
-  <si>
-    <t>Larceny-theft - Race</t>
-  </si>
-  <si>
-    <t>Larceny-theft - Religion</t>
-  </si>
-  <si>
-    <t>Larceny-theft - Sexual orientation</t>
-  </si>
-  <si>
-    <t>Larceny-theft - Gender</t>
-  </si>
-  <si>
-    <t>Larceny-theft - Disability</t>
-  </si>
-  <si>
-    <t>Larceny-theft - Ethnicity/National origin</t>
+    <t>Arson - Ethnicity/National Origin</t>
+  </si>
+  <si>
+    <t>Simple Assault</t>
+  </si>
+  <si>
+    <t>Simple Assault - Race</t>
+  </si>
+  <si>
+    <t>Simple Assault - Religion</t>
+  </si>
+  <si>
+    <t>Simple Assault - Sexual Orientation</t>
+  </si>
+  <si>
+    <t>Simple Assault - Gender</t>
+  </si>
+  <si>
+    <t>Simple Assault - Disability</t>
+  </si>
+  <si>
+    <t>Simple Assault - Ethnicity/National Origin</t>
+  </si>
+  <si>
+    <t>Larceny-Theft</t>
+  </si>
+  <si>
+    <t>Larceny-Theft - Race</t>
+  </si>
+  <si>
+    <t>Larceny-Theft - Religion</t>
+  </si>
+  <si>
+    <t>Larceny-Theft - Sexual Orientation</t>
+  </si>
+  <si>
+    <t>Larceny-Theft - Gender</t>
+  </si>
+  <si>
+    <t>Larceny-Theft - Disability</t>
+  </si>
+  <si>
+    <t>Larceny-Theft - Ethnicity/National Origin</t>
   </si>
   <si>
     <t>Intimidation</t>
@@ -274,7 +271,7 @@
     <t>Intimidation - Religion</t>
   </si>
   <si>
-    <t>Intimidation - Sexual orientation</t>
+    <t>Intimidation - Sexual Orientation</t>
   </si>
   <si>
     <t>Intimidation - Gender</t>
@@ -283,28 +280,28 @@
     <t>Intimidation - Disability</t>
   </si>
   <si>
-    <t>Intimidation - Ethnicity/National origin</t>
-  </si>
-  <si>
-    <t>Destruction/damage/ vandalism of property</t>
-  </si>
-  <si>
-    <t>Destruction/damage/ vandalism of property - Race</t>
-  </si>
-  <si>
-    <t>Destruction/damage/ vandalism of property - Religion</t>
-  </si>
-  <si>
-    <t>Destruction/damage/ vandalism of property - Sexual orientation</t>
-  </si>
-  <si>
-    <t>Destruction/damage/ vandalism of property - Gender</t>
-  </si>
-  <si>
-    <t>Destruction/damage/ vandalism of property - Disability</t>
-  </si>
-  <si>
-    <t>Destruction/damage/ vandalism of property - Ethnicity/National origin</t>
+    <t>Intimidation - Ethnicity/National Origin</t>
+  </si>
+  <si>
+    <t>Destruction/Damage/Vandalism of Property</t>
+  </si>
+  <si>
+    <t>Destruction/Damage/Vandalism of Property - Race</t>
+  </si>
+  <si>
+    <t>Destruction/Damage/Vandalism of Property - Religion</t>
+  </si>
+  <si>
+    <t>Destruction/Damage/Vandalism of Property - Sexual Orientation</t>
+  </si>
+  <si>
+    <t>Destruction/Damage/Vandalism of Property - Gender</t>
+  </si>
+  <si>
+    <t>Destruction/Damage/Vandalism of Property - Disability</t>
+  </si>
+  <si>
+    <t>Destruction/Damage/Vandalism of Property - Ethnicity/National Origin</t>
   </si>
   <si>
     <t>Bluefield College</t>
@@ -655,298 +652,343 @@
       <c t="s" s="1" r="A1">
         <v>0</v>
       </c>
+      <c t="s" s="1" r="B1">
+        <v>1</v>
+      </c>
+      <c t="s" s="1" r="C1">
+        <v>2</v>
+      </c>
+      <c t="s" s="1" r="D1">
+        <v>3</v>
+      </c>
+      <c t="s" s="1" r="E1">
+        <v>4</v>
+      </c>
+      <c t="s" s="1" r="F1">
+        <v>5</v>
+      </c>
+      <c t="s" s="1" r="G1">
+        <v>6</v>
+      </c>
+      <c t="s" s="1" r="H1">
+        <v>7</v>
+      </c>
+      <c t="s" s="1" r="I1">
+        <v>8</v>
+      </c>
+      <c t="s" s="1" r="J1">
+        <v>9</v>
+      </c>
+      <c t="s" s="1" r="K1">
+        <v>10</v>
+      </c>
+      <c t="s" s="1" r="L1">
+        <v>11</v>
+      </c>
+      <c t="s" s="1" r="M1">
+        <v>12</v>
+      </c>
+      <c t="s" s="1" r="N1">
+        <v>13</v>
+      </c>
+      <c t="s" s="1" r="O1">
+        <v>14</v>
+      </c>
+      <c t="s" s="1" r="P1">
+        <v>15</v>
+      </c>
+      <c t="s" s="1" r="Q1">
+        <v>16</v>
+      </c>
+      <c t="s" s="1" r="R1">
+        <v>17</v>
+      </c>
+      <c t="s" s="1" r="S1">
+        <v>18</v>
+      </c>
+      <c t="s" s="1" r="T1">
+        <v>19</v>
+      </c>
+      <c t="s" s="1" r="U1">
+        <v>20</v>
+      </c>
+      <c t="s" s="1" r="V1">
+        <v>21</v>
+      </c>
+      <c t="s" s="1" r="W1">
+        <v>22</v>
+      </c>
+      <c t="s" s="1" r="X1">
+        <v>23</v>
+      </c>
+      <c t="s" s="1" r="Y1">
+        <v>24</v>
+      </c>
+      <c t="s" s="1" r="Z1">
+        <v>25</v>
+      </c>
+      <c t="s" s="1" r="AA1">
+        <v>26</v>
+      </c>
+      <c t="s" s="1" r="AB1">
+        <v>27</v>
+      </c>
+      <c t="s" s="1" r="AC1">
+        <v>28</v>
+      </c>
+      <c t="s" s="1" r="AD1">
+        <v>29</v>
+      </c>
+      <c t="s" s="1" r="AE1">
+        <v>30</v>
+      </c>
+      <c t="s" s="1" r="AF1">
+        <v>31</v>
+      </c>
+      <c t="s" s="1" r="AG1">
+        <v>32</v>
+      </c>
+      <c t="s" s="1" r="AH1">
+        <v>33</v>
+      </c>
+      <c t="s" s="1" r="AI1">
+        <v>34</v>
+      </c>
+      <c t="s" s="1" r="AJ1">
+        <v>35</v>
+      </c>
+      <c t="s" s="1" r="AK1">
+        <v>36</v>
+      </c>
+      <c t="s" s="1" r="AL1">
+        <v>37</v>
+      </c>
+      <c t="s" s="1" r="AM1">
+        <v>38</v>
+      </c>
+      <c t="s" s="1" r="AN1">
+        <v>39</v>
+      </c>
+      <c t="s" s="1" r="AO1">
+        <v>40</v>
+      </c>
+      <c t="s" s="1" r="AP1">
+        <v>41</v>
+      </c>
+      <c t="s" s="1" r="AQ1">
+        <v>42</v>
+      </c>
+      <c t="s" s="1" r="AR1">
+        <v>43</v>
+      </c>
+      <c t="s" s="1" r="AS1">
+        <v>44</v>
+      </c>
+      <c t="s" s="1" r="AT1">
+        <v>45</v>
+      </c>
+      <c t="s" s="1" r="AU1">
+        <v>46</v>
+      </c>
+      <c t="s" s="1" r="AV1">
+        <v>47</v>
+      </c>
+      <c t="s" s="1" r="AW1">
+        <v>48</v>
+      </c>
+      <c t="s" s="1" r="AX1">
+        <v>49</v>
+      </c>
+      <c t="s" s="1" r="AY1">
+        <v>50</v>
+      </c>
+      <c t="s" s="1" r="AZ1">
+        <v>51</v>
+      </c>
+      <c t="s" s="1" r="BA1">
+        <v>52</v>
+      </c>
+      <c t="s" s="1" r="BB1">
+        <v>53</v>
+      </c>
+      <c t="s" s="1" r="BC1">
+        <v>54</v>
+      </c>
+      <c t="s" s="1" r="BD1">
+        <v>55</v>
+      </c>
+      <c t="s" s="1" r="BE1">
+        <v>56</v>
+      </c>
+      <c t="s" s="1" r="BF1">
+        <v>57</v>
+      </c>
+      <c t="s" s="1" r="BG1">
+        <v>58</v>
+      </c>
+      <c t="s" s="1" r="BH1">
+        <v>59</v>
+      </c>
+      <c t="s" s="1" r="BI1">
+        <v>60</v>
+      </c>
+      <c t="s" s="1" r="BJ1">
+        <v>61</v>
+      </c>
+      <c t="s" s="1" r="BK1">
+        <v>62</v>
+      </c>
+      <c t="s" s="1" r="BL1">
+        <v>63</v>
+      </c>
+      <c t="s" s="1" r="BM1">
+        <v>64</v>
+      </c>
+      <c t="s" s="1" r="BN1">
+        <v>65</v>
+      </c>
+      <c t="s" s="1" r="BO1">
+        <v>66</v>
+      </c>
+      <c t="s" s="1" r="BP1">
+        <v>67</v>
+      </c>
+      <c t="s" s="1" r="BQ1">
+        <v>68</v>
+      </c>
+      <c t="s" s="1" r="BR1">
+        <v>69</v>
+      </c>
+      <c t="s" s="1" r="BS1">
+        <v>70</v>
+      </c>
+      <c t="s" s="1" r="BT1">
+        <v>71</v>
+      </c>
+      <c t="s" s="1" r="BU1">
+        <v>72</v>
+      </c>
+      <c t="s" s="1" r="BV1">
+        <v>73</v>
+      </c>
+      <c t="s" s="1" r="BW1">
+        <v>74</v>
+      </c>
+      <c t="s" s="1" r="BX1">
+        <v>75</v>
+      </c>
+      <c t="s" s="1" r="BY1">
+        <v>76</v>
+      </c>
+      <c t="s" s="1" r="BZ1">
+        <v>77</v>
+      </c>
+      <c t="s" s="1" r="CA1">
+        <v>78</v>
+      </c>
+      <c t="s" s="1" r="CB1">
+        <v>79</v>
+      </c>
+      <c t="s" s="1" r="CC1">
+        <v>80</v>
+      </c>
+      <c t="s" s="1" r="CD1">
+        <v>81</v>
+      </c>
+      <c t="s" s="1" r="CE1">
+        <v>82</v>
+      </c>
+      <c t="s" s="1" r="CF1">
+        <v>83</v>
+      </c>
+      <c t="s" s="1" r="CG1">
+        <v>84</v>
+      </c>
+      <c t="s" s="1" r="CH1">
+        <v>85</v>
+      </c>
+      <c t="s" s="1" r="CI1">
+        <v>86</v>
+      </c>
+      <c t="s" s="1" r="CJ1">
+        <v>87</v>
+      </c>
+      <c t="s" s="1" r="CK1">
+        <v>88</v>
+      </c>
+      <c t="s" s="1" r="CL1">
+        <v>89</v>
+      </c>
+      <c t="s" s="1" r="CM1">
+        <v>90</v>
+      </c>
+      <c t="s" s="1" r="CN1">
+        <v>91</v>
+      </c>
+      <c t="s" s="1" r="CO1">
+        <v>92</v>
+      </c>
+      <c t="s" s="1" r="CP1">
+        <v>93</v>
+      </c>
+      <c t="s" s="1" r="CQ1">
+        <v>94</v>
+      </c>
+      <c t="s" s="1" r="CR1">
+        <v>95</v>
+      </c>
+      <c t="s" s="1" r="CS1">
+        <v>96</v>
+      </c>
     </row>
     <row r="2">
-      <c t="s" s="1" r="A2">
-        <v>1</v>
-      </c>
-      <c t="s" s="1" r="B2">
-        <v>2</v>
+      <c s="1" r="A2">
+        <v>2003.0</v>
+      </c>
+      <c s="1" r="B2">
+        <v>231554.0</v>
       </c>
       <c t="s" s="1" r="C2">
-        <v>3</v>
-      </c>
-      <c t="s" s="1" r="D2">
-        <v>4</v>
+        <v>97</v>
+      </c>
+      <c s="1" r="D2">
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E2">
-        <v>5</v>
-      </c>
-      <c t="s" s="1" r="F2">
-        <v>6</v>
-      </c>
-      <c t="s" s="1" r="G2">
-        <v>7</v>
-      </c>
-      <c t="s" s="1" r="H2">
-        <v>8</v>
-      </c>
-      <c t="s" s="1" r="I2">
-        <v>9</v>
-      </c>
-      <c t="s" s="1" r="J2">
-        <v>10</v>
-      </c>
-      <c t="s" s="1" r="K2">
-        <v>11</v>
-      </c>
-      <c t="s" s="1" r="L2">
-        <v>12</v>
-      </c>
-      <c t="s" s="1" r="M2">
-        <v>13</v>
-      </c>
-      <c t="s" s="1" r="N2">
-        <v>14</v>
-      </c>
-      <c t="s" s="1" r="O2">
-        <v>15</v>
-      </c>
-      <c t="s" s="1" r="P2">
-        <v>16</v>
-      </c>
-      <c t="s" s="1" r="Q2">
-        <v>17</v>
-      </c>
-      <c t="s" s="1" r="R2">
-        <v>18</v>
-      </c>
-      <c t="s" s="1" r="S2">
-        <v>19</v>
-      </c>
-      <c t="s" s="1" r="T2">
-        <v>20</v>
-      </c>
-      <c t="s" s="1" r="U2">
-        <v>21</v>
-      </c>
-      <c t="s" s="1" r="V2">
-        <v>22</v>
-      </c>
-      <c t="s" s="1" r="W2">
-        <v>23</v>
-      </c>
-      <c t="s" s="1" r="X2">
-        <v>24</v>
-      </c>
-      <c t="s" s="1" r="Y2">
-        <v>25</v>
-      </c>
-      <c t="s" s="1" r="Z2">
-        <v>26</v>
-      </c>
-      <c t="s" s="1" r="AA2">
-        <v>27</v>
-      </c>
-      <c t="s" s="1" r="AB2">
-        <v>28</v>
-      </c>
-      <c t="s" s="1" r="AC2">
-        <v>29</v>
-      </c>
-      <c t="s" s="1" r="AD2">
-        <v>30</v>
-      </c>
-      <c t="s" s="1" r="AE2">
-        <v>31</v>
-      </c>
-      <c t="s" s="1" r="AF2">
-        <v>32</v>
-      </c>
-      <c t="s" s="1" r="AG2">
-        <v>33</v>
-      </c>
-      <c t="s" s="1" r="AH2">
-        <v>34</v>
-      </c>
-      <c t="s" s="1" r="AI2">
-        <v>35</v>
-      </c>
-      <c t="s" s="1" r="AJ2">
-        <v>36</v>
-      </c>
-      <c t="s" s="1" r="AK2">
-        <v>37</v>
-      </c>
-      <c t="s" s="1" r="AL2">
-        <v>38</v>
-      </c>
-      <c t="s" s="1" r="AM2">
-        <v>39</v>
-      </c>
-      <c t="s" s="1" r="AN2">
-        <v>40</v>
-      </c>
-      <c t="s" s="1" r="AO2">
-        <v>41</v>
-      </c>
-      <c t="s" s="1" r="AP2">
-        <v>42</v>
-      </c>
-      <c t="s" s="1" r="AQ2">
-        <v>43</v>
-      </c>
-      <c t="s" s="1" r="AR2">
-        <v>44</v>
-      </c>
-      <c t="s" s="1" r="AS2">
-        <v>45</v>
-      </c>
-      <c t="s" s="1" r="AT2">
-        <v>46</v>
-      </c>
-      <c t="s" s="1" r="AU2">
-        <v>47</v>
-      </c>
-      <c t="s" s="1" r="AV2">
-        <v>48</v>
-      </c>
-      <c t="s" s="1" r="AW2">
-        <v>49</v>
-      </c>
-      <c t="s" s="1" r="AX2">
-        <v>50</v>
-      </c>
-      <c t="s" s="1" r="AY2">
-        <v>51</v>
-      </c>
-      <c t="s" s="1" r="AZ2">
-        <v>52</v>
-      </c>
-      <c t="s" s="1" r="BA2">
-        <v>53</v>
-      </c>
-      <c t="s" s="1" r="BB2">
-        <v>54</v>
-      </c>
-      <c t="s" s="1" r="BC2">
-        <v>55</v>
-      </c>
-      <c t="s" s="1" r="BD2">
-        <v>56</v>
-      </c>
-      <c t="s" s="1" r="BE2">
-        <v>57</v>
-      </c>
-      <c t="s" s="1" r="BF2">
-        <v>58</v>
-      </c>
-      <c t="s" s="1" r="BG2">
-        <v>59</v>
-      </c>
-      <c t="s" s="1" r="BH2">
-        <v>60</v>
-      </c>
-      <c t="s" s="1" r="BI2">
-        <v>61</v>
-      </c>
-      <c t="s" s="1" r="BJ2">
-        <v>62</v>
-      </c>
-      <c t="s" s="1" r="BK2">
-        <v>63</v>
-      </c>
-      <c t="s" s="1" r="BL2">
-        <v>64</v>
-      </c>
-      <c t="s" s="1" r="BM2">
-        <v>65</v>
-      </c>
-      <c t="s" s="1" r="BN2">
-        <v>66</v>
-      </c>
-      <c t="s" s="1" r="BO2">
-        <v>67</v>
-      </c>
-      <c t="s" s="1" r="BP2">
-        <v>68</v>
-      </c>
-      <c t="s" s="1" r="BQ2">
-        <v>69</v>
-      </c>
-      <c t="s" s="1" r="BR2">
-        <v>70</v>
-      </c>
-      <c t="s" s="1" r="BS2">
-        <v>71</v>
-      </c>
-      <c t="s" s="1" r="BT2">
-        <v>72</v>
-      </c>
-      <c t="s" s="1" r="BU2">
-        <v>73</v>
-      </c>
-      <c t="s" s="1" r="BV2">
-        <v>74</v>
-      </c>
-      <c t="s" s="1" r="BW2">
-        <v>75</v>
-      </c>
-      <c t="s" s="1" r="BX2">
-        <v>76</v>
-      </c>
-      <c t="s" s="1" r="BY2">
-        <v>77</v>
-      </c>
-      <c t="s" s="1" r="BZ2">
-        <v>78</v>
-      </c>
-      <c t="s" s="1" r="CA2">
-        <v>79</v>
-      </c>
-      <c t="s" s="1" r="CB2">
-        <v>80</v>
-      </c>
-      <c t="s" s="1" r="CC2">
-        <v>81</v>
-      </c>
-      <c t="s" s="1" r="CD2">
-        <v>82</v>
-      </c>
-      <c t="s" s="1" r="CE2">
-        <v>83</v>
-      </c>
-      <c t="s" s="1" r="CF2">
-        <v>84</v>
-      </c>
-      <c t="s" s="1" r="CG2">
-        <v>85</v>
-      </c>
-      <c t="s" s="1" r="CH2">
-        <v>86</v>
-      </c>
-      <c t="s" s="1" r="CI2">
-        <v>87</v>
-      </c>
-      <c t="s" s="1" r="CJ2">
-        <v>88</v>
-      </c>
-      <c t="s" s="1" r="CK2">
-        <v>89</v>
-      </c>
-      <c t="s" s="1" r="CL2">
-        <v>90</v>
-      </c>
-      <c t="s" s="1" r="CM2">
-        <v>91</v>
-      </c>
-      <c t="s" s="1" r="CN2">
-        <v>92</v>
-      </c>
-      <c t="s" s="1" r="CO2">
-        <v>93</v>
-      </c>
-      <c t="s" s="1" r="CP2">
-        <v>94</v>
-      </c>
-      <c t="s" s="1" r="CQ2">
-        <v>95</v>
-      </c>
-      <c t="s" s="1" r="CR2">
-        <v>96</v>
-      </c>
-      <c t="s" s="1" r="CS2">
-        <v>97</v>
+        <v>98</v>
+      </c>
+      <c s="1" r="F2">
+        <v>731.0</v>
+      </c>
+      <c s="1" r="G2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="N2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="U2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="AB2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="AI2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="AP2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="AW2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="BD2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="BK2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="BR2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -954,19 +996,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B3">
-        <v>231554.0</v>
+        <v>231712.0</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c s="1" r="D3">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E3">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c s="1" r="F3">
-        <v>731.0</v>
+        <v>4812.0</v>
       </c>
       <c s="1" r="G3">
         <v>0.0</v>
@@ -1004,19 +1046,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B4">
-        <v>231712.0</v>
+        <v>231624.0</v>
       </c>
       <c t="s" s="1" r="C4">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c s="1" r="D4">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E4">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c s="1" r="F4">
-        <v>4812.0</v>
+        <v>7749.0</v>
       </c>
       <c s="1" r="G4">
         <v>0.0</v>
@@ -1054,19 +1096,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B5">
-        <v>231624.0</v>
+        <v>231970.0</v>
       </c>
       <c t="s" s="1" r="C5">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c s="1" r="D5">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E5">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c s="1" r="F5">
-        <v>7749.0</v>
+        <v>638.0</v>
       </c>
       <c s="1" r="G5">
         <v>0.0</v>
@@ -1104,19 +1146,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B6">
-        <v>231970.0</v>
+        <v>442806.0</v>
       </c>
       <c t="s" s="1" r="C6">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c s="1" r="D6">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E6">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c s="1" r="F6">
-        <v>638.0</v>
+        <v>154.0</v>
       </c>
       <c s="1" r="G6">
         <v>0.0</v>
@@ -1154,19 +1196,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B7">
-        <v>442806.0</v>
+        <v>232089.0</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c s="1" r="D7">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E7">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c s="1" r="F7">
-        <v>154.0</v>
+        <v>954.0</v>
       </c>
       <c s="1" r="G7">
         <v>0.0</v>
@@ -1204,19 +1246,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B8">
-        <v>232089.0</v>
+        <v>232186.0</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c s="1" r="D8">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E8">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c s="1" r="F8">
-        <v>954.0</v>
+        <v>28246.0</v>
       </c>
       <c s="1" r="G8">
         <v>0.0</v>
@@ -1254,19 +1296,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B9">
-        <v>232186.0</v>
+        <v>232256.0</v>
       </c>
       <c t="s" s="1" r="C9">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c s="1" r="D9">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E9">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c s="1" r="F9">
-        <v>28246.0</v>
+        <v>1039.0</v>
       </c>
       <c s="1" r="G9">
         <v>0.0</v>
@@ -1304,19 +1346,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B10">
-        <v>232256.0</v>
+        <v>232423.0</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c s="1" r="D10">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E10">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c s="1" r="F10">
-        <v>1039.0</v>
+        <v>16203.0</v>
       </c>
       <c s="1" r="G10">
         <v>0.0</v>
@@ -1357,13 +1399,13 @@
         <v>232423.0</v>
       </c>
       <c t="s" s="1" r="C11">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c s="1" r="D11">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c t="s" s="1" r="E11">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c s="1" r="F11">
         <v>16203.0</v>
@@ -1404,19 +1446,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B12">
-        <v>232423.0</v>
+        <v>232566.0</v>
       </c>
       <c t="s" s="1" r="C12">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c s="1" r="D12">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E12">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c s="1" r="F12">
-        <v>16203.0</v>
+        <v>4252.0</v>
       </c>
       <c s="1" r="G12">
         <v>0.0</v>
@@ -1454,19 +1496,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B13">
-        <v>232566.0</v>
+        <v>232609.0</v>
       </c>
       <c t="s" s="1" r="C13">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c s="1" r="D13">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E13">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c s="1" r="F13">
-        <v>4252.0</v>
+        <v>2009.0</v>
       </c>
       <c s="1" r="G13">
         <v>0.0</v>
@@ -1504,19 +1546,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B14">
-        <v>232609.0</v>
+        <v>232706.0</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c s="1" r="D14">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E14">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c s="1" r="F14">
-        <v>2009.0</v>
+        <v>3741.0</v>
       </c>
       <c s="1" r="G14">
         <v>0.0</v>
@@ -1554,19 +1596,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B15">
-        <v>232706.0</v>
+        <v>232788.0</v>
       </c>
       <c t="s" s="1" r="C15">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c s="1" r="D15">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E15">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c s="1" r="F15">
-        <v>3741.0</v>
+        <v>2875.0</v>
       </c>
       <c s="1" r="G15">
         <v>0.0</v>
@@ -1604,19 +1646,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B16">
-        <v>232788.0</v>
+        <v>232867.0</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c s="1" r="D16">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E16">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c s="1" r="F16">
-        <v>2875.0</v>
+        <v>4327.0</v>
       </c>
       <c s="1" r="G16">
         <v>0.0</v>
@@ -1654,19 +1696,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B17">
-        <v>232867.0</v>
+        <v>433299.0</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c s="1" r="D17">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E17">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c s="1" r="F17">
-        <v>4327.0</v>
+        <v>52.0</v>
       </c>
       <c s="1" r="G17">
         <v>0.0</v>
@@ -1704,19 +1746,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B18">
-        <v>433299.0</v>
+        <v>233417.0</v>
       </c>
       <c t="s" s="1" r="C18">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c s="1" r="D18">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E18">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c s="1" r="F18">
-        <v>52.0</v>
+        <v>45.0</v>
       </c>
       <c s="1" r="G18">
         <v>0.0</v>
@@ -1754,19 +1796,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B19">
-        <v>233417.0</v>
+        <v>232937.0</v>
       </c>
       <c t="s" s="1" r="C19">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c s="1" r="D19">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E19">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c s="1" r="F19">
-        <v>45.0</v>
+        <v>6846.0</v>
       </c>
       <c s="1" r="G19">
         <v>0.0</v>
@@ -1804,19 +1846,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B20">
-        <v>232937.0</v>
+        <v>232946.0</v>
       </c>
       <c t="s" s="1" r="C20">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c s="1" r="D20">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E20">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c s="1" r="F20">
-        <v>6846.0</v>
+        <v>38097.0</v>
       </c>
       <c s="1" r="G20">
         <v>0.0</v>
@@ -1857,13 +1899,13 @@
         <v>232946.0</v>
       </c>
       <c t="s" s="1" r="C21">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c s="1" r="D21">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c t="s" s="1" r="E21">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c s="1" r="F21">
         <v>38097.0</v>
@@ -1907,13 +1949,13 @@
         <v>232946.0</v>
       </c>
       <c t="s" s="1" r="C22">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c s="1" r="D22">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c t="s" s="1" r="E22">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c s="1" r="F22">
         <v>38097.0</v>
@@ -1957,13 +1999,13 @@
         <v>232946.0</v>
       </c>
       <c t="s" s="1" r="C23">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c s="1" r="D23">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c t="s" s="1" r="E23">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c s="1" r="F23">
         <v>38097.0</v>
@@ -2004,19 +2046,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B24">
-        <v>232946.0</v>
+        <v>232982.0</v>
       </c>
       <c t="s" s="1" r="C24">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c s="1" r="D24">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E24">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c s="1" r="F24">
-        <v>38097.0</v>
+        <v>20802.0</v>
       </c>
       <c s="1" r="G24">
         <v>0.0</v>
@@ -2054,19 +2096,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B25">
-        <v>232982.0</v>
+        <v>233019.0</v>
       </c>
       <c t="s" s="1" r="C25">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c s="1" r="D25">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E25">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c s="1" r="F25">
-        <v>20802.0</v>
+        <v>3492.0</v>
       </c>
       <c s="1" r="G25">
         <v>0.0</v>
@@ -2104,19 +2146,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B26">
-        <v>233019.0</v>
+        <v>233277.0</v>
       </c>
       <c t="s" s="1" r="C26">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c s="1" r="D26">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E26">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c s="1" r="F26">
-        <v>3492.0</v>
+        <v>9219.0</v>
       </c>
       <c s="1" r="G26">
         <v>0.0</v>
@@ -2154,19 +2196,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B27">
-        <v>233277.0</v>
+        <v>437769.0</v>
       </c>
       <c t="s" s="1" r="C27">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c s="1" r="D27">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E27">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c s="1" r="F27">
-        <v>9219.0</v>
+        <v>480.0</v>
       </c>
       <c s="1" r="G27">
         <v>0.0</v>
@@ -2204,19 +2246,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B28">
-        <v>437769.0</v>
+        <v>233408.0</v>
       </c>
       <c t="s" s="1" r="C28">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c s="1" r="D28">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E28">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c s="1" r="F28">
-        <v>480.0</v>
+        <v>154.0</v>
       </c>
       <c s="1" r="G28">
         <v>0.0</v>
@@ -2254,19 +2296,16 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B29">
-        <v>233408.0</v>
+        <v>435213.0</v>
       </c>
       <c t="s" s="1" r="C29">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c s="1" r="D29">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E29">
-        <v>151</v>
-      </c>
-      <c s="1" r="F29">
-        <v>154.0</v>
+        <v>152</v>
       </c>
       <c s="1" r="G29">
         <v>0.0</v>
@@ -2304,16 +2343,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B30">
-        <v>435213.0</v>
+        <v>233499.0</v>
       </c>
       <c t="s" s="1" r="C30">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c s="1" r="D30">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E30">
-        <v>153</v>
+        <v>154</v>
+      </c>
+      <c s="1" r="F30">
+        <v>475.0</v>
       </c>
       <c s="1" r="G30">
         <v>0.0</v>
@@ -2351,19 +2393,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B31">
-        <v>233499.0</v>
+        <v>233541.0</v>
       </c>
       <c t="s" s="1" r="C31">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c s="1" r="D31">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E31">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c s="1" r="F31">
-        <v>475.0</v>
+        <v>2851.0</v>
       </c>
       <c s="1" r="G31">
         <v>0.0</v>
@@ -2401,19 +2443,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B32">
-        <v>233541.0</v>
+        <v>233639.0</v>
       </c>
       <c t="s" s="1" r="C32">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c s="1" r="D32">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E32">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c s="1" r="F32">
-        <v>2851.0</v>
+        <v>4894.0</v>
       </c>
       <c s="1" r="G32">
         <v>0.0</v>
@@ -2451,19 +2493,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B33">
-        <v>233639.0</v>
+        <v>440341.0</v>
       </c>
       <c t="s" s="1" r="C33">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c s="1" r="D33">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E33">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c s="1" r="F33">
-        <v>4894.0</v>
+        <v>852.0</v>
       </c>
       <c s="1" r="G33">
         <v>0.0</v>
@@ -2501,19 +2543,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B34">
-        <v>440341.0</v>
+        <v>233897.0</v>
       </c>
       <c t="s" s="1" r="C34">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c s="1" r="D34">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E34">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c s="1" r="F34">
-        <v>852.0</v>
+        <v>1703.0</v>
       </c>
       <c s="1" r="G34">
         <v>0.0</v>
@@ -2551,19 +2593,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B35">
-        <v>233897.0</v>
+        <v>233754.0</v>
       </c>
       <c t="s" s="1" r="C35">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c s="1" r="D35">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E35">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c s="1" r="F35">
-        <v>1703.0</v>
+        <v>7889.0</v>
       </c>
       <c s="1" r="G35">
         <v>0.0</v>
@@ -2601,19 +2643,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B36">
-        <v>233754.0</v>
+        <v>233772.0</v>
       </c>
       <c t="s" s="1" r="C36">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c s="1" r="D36">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c t="s" s="1" r="E36">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c s="1" r="F36">
-        <v>7889.0</v>
+        <v>23088.0</v>
       </c>
       <c s="1" r="G36">
         <v>0.0</v>
@@ -2651,19 +2693,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B37">
-        <v>233772.0</v>
+        <v>232681.0</v>
       </c>
       <c t="s" s="1" r="C37">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c s="1" r="D37">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E37">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c s="1" r="F37">
-        <v>23088.0</v>
+        <v>4792.0</v>
       </c>
       <c s="1" r="G37">
         <v>0.0</v>
@@ -2701,19 +2743,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B38">
-        <v>232681.0</v>
+        <v>233374.0</v>
       </c>
       <c t="s" s="1" r="C38">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c s="1" r="D38">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E38">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c s="1" r="F38">
-        <v>4792.0</v>
+        <v>4444.0</v>
       </c>
       <c s="1" r="G38">
         <v>0.0</v>
@@ -2751,19 +2793,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B39">
-        <v>233374.0</v>
+        <v>234076.0</v>
       </c>
       <c t="s" s="1" r="C39">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c s="1" r="D39">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E39">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c s="1" r="F39">
-        <v>4444.0</v>
+        <v>23077.0</v>
       </c>
       <c s="1" r="G39">
         <v>0.0</v>
@@ -2793,7 +2835,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="BR39">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="40">
@@ -2801,19 +2843,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B40">
-        <v>234076.0</v>
+        <v>234030.0</v>
       </c>
       <c t="s" s="1" r="C40">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c s="1" r="D40">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E40">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c s="1" r="F40">
-        <v>23077.0</v>
+        <v>26631.0</v>
       </c>
       <c s="1" r="G40">
         <v>0.0</v>
@@ -2843,7 +2885,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="BR40">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="41">
@@ -2854,13 +2896,13 @@
         <v>234030.0</v>
       </c>
       <c t="s" s="1" r="C41">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c s="1" r="D41">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c t="s" s="1" r="E41">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c s="1" r="F41">
         <v>26631.0</v>
@@ -2901,19 +2943,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B42">
-        <v>234030.0</v>
+        <v>233912.0</v>
       </c>
       <c t="s" s="1" r="C42">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c s="1" r="D42">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E42">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c s="1" r="F42">
-        <v>26631.0</v>
+        <v>1124.0</v>
       </c>
       <c s="1" r="G42">
         <v>0.0</v>
@@ -2927,16 +2969,7 @@
       <c s="1" r="AB42">
         <v>0.0</v>
       </c>
-      <c s="1" r="AI42">
-        <v>0.0</v>
-      </c>
       <c s="1" r="AP42">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="AW42">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="BD42">
         <v>0.0</v>
       </c>
       <c s="1" r="BK42">
@@ -2951,19 +2984,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B43">
-        <v>233912.0</v>
+        <v>234085.0</v>
       </c>
       <c t="s" s="1" r="C43">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c s="1" r="D43">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E43">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c s="1" r="F43">
-        <v>1124.0</v>
+        <v>1333.0</v>
       </c>
       <c s="1" r="G43">
         <v>0.0</v>
@@ -2977,7 +3010,16 @@
       <c s="1" r="AB43">
         <v>0.0</v>
       </c>
+      <c s="1" r="AI43">
+        <v>0.0</v>
+      </c>
       <c s="1" r="AP43">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="AW43">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="BD43">
         <v>0.0</v>
       </c>
       <c s="1" r="BK43">
@@ -2992,19 +3034,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B44">
-        <v>234085.0</v>
+        <v>233921.0</v>
       </c>
       <c t="s" s="1" r="C44">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c s="1" r="D44">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E44">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c s="1" r="F44">
-        <v>1333.0</v>
+        <v>27755.0</v>
       </c>
       <c s="1" r="G44">
         <v>0.0</v>
@@ -3018,16 +3060,7 @@
       <c s="1" r="AB44">
         <v>0.0</v>
       </c>
-      <c s="1" r="AI44">
-        <v>0.0</v>
-      </c>
       <c s="1" r="AP44">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="AW44">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="BD44">
         <v>0.0</v>
       </c>
       <c s="1" r="BK44">
@@ -3042,19 +3075,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B45">
-        <v>233921.0</v>
+        <v>234155.0</v>
       </c>
       <c t="s" s="1" r="C45">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c s="1" r="D45">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E45">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c s="1" r="F45">
-        <v>27755.0</v>
+        <v>4933.0</v>
       </c>
       <c s="1" r="G45">
         <v>0.0</v>
@@ -3068,7 +3101,16 @@
       <c s="1" r="AB45">
         <v>0.0</v>
       </c>
+      <c s="1" r="AI45">
+        <v>0.0</v>
+      </c>
       <c s="1" r="AP45">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="AW45">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="BD45">
         <v>0.0</v>
       </c>
       <c s="1" r="BK45">
@@ -3083,19 +3125,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B46">
-        <v>234155.0</v>
+        <v>233949.0</v>
       </c>
       <c t="s" s="1" r="C46">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c s="1" r="D46">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E46">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c s="1" r="F46">
-        <v>4933.0</v>
+        <v>8124.0</v>
       </c>
       <c s="1" r="G46">
         <v>0.0</v>
@@ -3133,19 +3175,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B47">
-        <v>233949.0</v>
+        <v>234207.0</v>
       </c>
       <c t="s" s="1" r="C47">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c s="1" r="D47">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E47">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c s="1" r="F47">
-        <v>8124.0</v>
+        <v>2137.0</v>
       </c>
       <c s="1" r="G47">
         <v>0.0</v>
@@ -3183,19 +3225,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B48">
-        <v>234207.0</v>
+        <v>234377.0</v>
       </c>
       <c t="s" s="1" r="C48">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c s="1" r="D48">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E48">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c s="1" r="F48">
-        <v>2137.0</v>
+        <v>2948.0</v>
       </c>
       <c s="1" r="G48">
         <v>0.0</v>
@@ -3225,56 +3267,6 @@
         <v>0.0</v>
       </c>
       <c s="1" r="BR48">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="49">
-      <c s="1" r="A49">
-        <v>2003.0</v>
-      </c>
-      <c s="1" r="B49">
-        <v>234377.0</v>
-      </c>
-      <c t="s" s="1" r="C49">
-        <v>190</v>
-      </c>
-      <c s="1" r="D49">
-        <v>1.0</v>
-      </c>
-      <c t="s" s="1" r="E49">
-        <v>191</v>
-      </c>
-      <c s="1" r="F49">
-        <v>2948.0</v>
-      </c>
-      <c s="1" r="G49">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="N49">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="U49">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="AB49">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="AI49">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="AP49">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="AW49">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="BD49">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="BK49">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="BR49">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>